<commit_message>
rewrite MCDA performance score calculation, update results
</commit_message>
<xml_diff>
--- a/dmsan/bwaise/scores/other_indicator_scores.xlsx
+++ b/dmsan/bwaise/scores/other_indicator_scores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yalinli_cabbi/Library/CloudStorage/OneDrive-Personal/Coding/ds/dmsan/bwaise/scores/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yalinli_cabbi/Code/DMsan/dmsan/bwaise/scores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34FACFC-BA94-FA42-8D65-08B83EE34530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824B1528-2B1A-2145-8FE2-A9140CCFAAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="11420" windowWidth="28800" windowHeight="15880" firstSheet="6" activeTab="11" xr2:uid="{672D30C3-4BC8-BB41-BA04-8F7D3B55B551}"/>
+    <workbookView xWindow="3080" yWindow="11420" windowWidth="28800" windowHeight="15880" xr2:uid="{672D30C3-4BC8-BB41-BA04-8F7D3B55B551}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSummary" sheetId="25" r:id="rId1"/>
@@ -954,7 +954,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1008,6 +1008,13 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1075,7 +1082,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1090,9 +1097,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1412,8 +1421,8 @@
   </sheetPr>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1424,8 +1433,8 @@
     <col min="4" max="4" width="15.1640625" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.1640625" style="13" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" style="18" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="15" customWidth="1"/>
     <col min="9" max="16384" width="8.6640625" style="13"/>
   </cols>
   <sheetData>
@@ -1448,7 +1457,7 @@
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="16" t="s">
         <v>89</v>
       </c>
       <c r="H1" s="13"/>
@@ -1472,7 +1481,7 @@
       <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1495,7 +1504,7 @@
       <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1518,7 +1527,7 @@
       <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1541,7 +1550,7 @@
       <c r="F5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1564,7 +1573,7 @@
       <c r="F6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1587,7 +1596,7 @@
       <c r="F7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1682,10 +1691,10 @@
       <c r="F11" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="G11" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="15"/>
+      <c r="G11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="14"/>
     </row>
     <row r="12" spans="1:8" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
@@ -1709,7 +1718,7 @@
       <c r="G12" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="H12" s="15"/>
+      <c r="H12" s="14"/>
     </row>
     <row r="13" spans="1:8" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
@@ -1733,7 +1742,7 @@
       <c r="G13" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="H13" s="15"/>
+      <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:8" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
@@ -1757,7 +1766,7 @@
       <c r="G14" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="H14" s="15"/>
+      <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:8" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
@@ -1781,7 +1790,7 @@
       <c r="G15" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="H15" s="15"/>
+      <c r="H15" s="14"/>
     </row>
     <row r="16" spans="1:8" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
@@ -1805,7 +1814,7 @@
       <c r="G16" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="15"/>
+      <c r="H16" s="14"/>
     </row>
     <row r="17" spans="1:8" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
@@ -1826,7 +1835,7 @@
       <c r="F17" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="5" t="s">
         <v>198</v>
       </c>
       <c r="H17" s="11"/>
@@ -1850,7 +1859,7 @@
       <c r="F18" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="5" t="s">
         <v>198</v>
       </c>
       <c r="H18" s="11"/>
@@ -1874,7 +1883,7 @@
       <c r="F19" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="5" t="s">
         <v>198</v>
       </c>
       <c r="H19" s="11"/>
@@ -1898,7 +1907,7 @@
       <c r="F20" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="17" t="s">
         <v>198</v>
       </c>
     </row>
@@ -1921,7 +1930,7 @@
       <c r="F21" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="9" t="s">
         <v>197</v>
       </c>
       <c r="H21" s="8"/>
@@ -1945,7 +1954,7 @@
       <c r="F22" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="9" t="s">
         <v>16</v>
       </c>
       <c r="H22" s="8"/>
@@ -1969,7 +1978,7 @@
       <c r="F23" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="9" t="s">
         <v>197</v>
       </c>
     </row>
@@ -1992,7 +2001,7 @@
       <c r="F24" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="9" t="s">
         <v>16</v>
       </c>
       <c r="H24" s="8"/>
@@ -2016,7 +2025,7 @@
       <c r="F25" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="9" t="s">
         <v>197</v>
       </c>
     </row>
@@ -2039,7 +2048,7 @@
       <c r="F26" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2062,7 +2071,7 @@
       <c r="F27" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G27" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2085,7 +2094,7 @@
       <c r="F28" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G28" s="9" t="s">
         <v>16</v>
       </c>
       <c r="H28" s="8"/>
@@ -2109,7 +2118,7 @@
       <c r="F29" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G29" s="9" t="s">
         <v>16</v>
       </c>
       <c r="H29" s="8"/>
@@ -2388,8 +2397,8 @@
   </sheetPr>
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>